<commit_message>
Updated face API response
</commit_message>
<xml_diff>
--- a/hello/CustomerData.xlsx
+++ b/hello/CustomerData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -481,6 +481,42 @@
         </is>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Kots</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>images/kotesh.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Kots</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>images/kotesh.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Kots</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>images/kotesh.png</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated face and register apis
</commit_message>
<xml_diff>
--- a/hello/CustomerData.xlsx
+++ b/hello/CustomerData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -517,6 +517,18 @@
         </is>
       </c>
     </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Doe</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>D:\Robot\myproject\hello\images/p2.JPG</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Added relative path for updated register api
</commit_message>
<xml_diff>
--- a/hello/CustomerData.xlsx
+++ b/hello/CustomerData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,60 +472,12 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Kots</t>
+          <t>Doe</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>images/kotesh.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Kots</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>images/kotesh.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Kots</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>images/kotesh.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>Kots</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>images/kotesh.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>Doe</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>D:\Robot\myproject\hello\images/p2.JPG</t>
+          <t>images/charan.jpeg</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated all the apis with relative path
</commit_message>
<xml_diff>
--- a/hello/CustomerData.xlsx
+++ b/hello/CustomerData.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -448,36 +448,24 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Vagdevi</t>
+          <t>Koti</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>images/Vagdevi(photo).png</t>
+          <t>images/kotesh.png</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Kots</t>
+          <t>Vaggg</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>images/kotesh.png</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Doe</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>images/charan.jpeg</t>
+          <t>images/Vagdevi(photo).png</t>
         </is>
       </c>
     </row>

</xml_diff>